<commit_message>
Enable return into game from any card, even if start outside of game
</commit_message>
<xml_diff>
--- a/data/all_cards.xlsx
+++ b/data/all_cards.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$35</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>city</t>
   </si>
@@ -76,6 +79,87 @@
   </si>
   <si>
     <t>Lima</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Moscou</t>
+  </si>
+  <si>
+    <t>Saint-Petersbourg</t>
+  </si>
+  <si>
+    <t>Francfort</t>
+  </si>
+  <si>
+    <t>Bogota</t>
+  </si>
+  <si>
+    <t>Santiago</t>
+  </si>
+  <si>
+    <t>Kinshasa</t>
+  </si>
+  <si>
+    <t>Antananarivo</t>
+  </si>
+  <si>
+    <t>Dar es Salam</t>
+  </si>
+  <si>
+    <t>Khartoum</t>
+  </si>
+  <si>
+    <t>Johannesburg</t>
+  </si>
+  <si>
+    <t>Bagdad</t>
+  </si>
+  <si>
+    <t>Teheran</t>
+  </si>
+  <si>
+    <t>Riyad</t>
+  </si>
+  <si>
+    <t>Dehli</t>
+  </si>
+  <si>
+    <t>Calcutta</t>
+  </si>
+  <si>
+    <t>Navi Mumbai</t>
+  </si>
+  <si>
+    <t>original</t>
+  </si>
+  <si>
+    <t>Jakarta</t>
+  </si>
+  <si>
+    <t>Bankok</t>
+  </si>
+  <si>
+    <t>Ho-Chi-Minh-Ville</t>
+  </si>
+  <si>
+    <t>Manille</t>
+  </si>
+  <si>
+    <t>Seoul</t>
+  </si>
+  <si>
+    <t>Tokyo</t>
+  </si>
+  <si>
+    <t>Osaka</t>
+  </si>
+  <si>
+    <t>Shanghai</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
   </si>
 </sst>
 </file>
@@ -403,24 +487,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -428,7 +517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -436,7 +525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -444,7 +533,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -452,23 +541,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -476,7 +571,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -484,7 +579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -492,7 +587,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -500,7 +595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -508,7 +603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -516,7 +611,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -524,7 +619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -532,31 +627,246 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B35"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
enable epidemic with bottom card coming from reserve
</commit_message>
<xml_diff>
--- a/data/all_cards.xlsx
+++ b/data/all_cards.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$45</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,14 +22,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>city</t>
   </si>
   <si>
-    <t>count</t>
-  </si>
-  <si>
     <t>Istanbul</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     <t>Navi Mumbai</t>
   </si>
   <si>
-    <t>original</t>
-  </si>
-  <si>
     <t>Jakarta</t>
   </si>
   <si>
@@ -160,6 +154,18 @@
   </si>
   <si>
     <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>Hommes-creux</t>
+  </si>
+  <si>
+    <t>in_reserve</t>
+  </si>
+  <si>
+    <t>in_discard</t>
+  </si>
+  <si>
+    <t>in_deck</t>
   </si>
 </sst>
 </file>
@@ -487,386 +493,652 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B8">
         <v>2</v>
       </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B19">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B26">
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B30">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B44">
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B35"/>
+  <autoFilter ref="A1:D45"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
cities update end October
</commit_message>
<xml_diff>
--- a/data/all_cards.xlsx
+++ b/data/all_cards.xlsx
@@ -132,9 +132,6 @@
     <t>Jakarta</t>
   </si>
   <si>
-    <t>Bankok</t>
-  </si>
-  <si>
     <t>Ho-Chi-Minh-Ville</t>
   </si>
   <si>
@@ -166,6 +163,9 @@
   </si>
   <si>
     <t>in_deck</t>
+  </si>
+  <si>
+    <t>Bangkok</t>
   </si>
 </sst>
 </file>
@@ -495,9 +495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -512,18 +510,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -568,7 +566,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -610,10 +608,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -750,10 +748,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -890,7 +888,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -974,7 +972,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1027,10 +1025,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1041,10 +1039,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1055,10 +1053,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1069,10 +1067,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1083,10 +1081,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -1097,10 +1095,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1111,10 +1109,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -1125,10 +1123,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C45">
         <v>0</v>

</xml_diff>

<commit_message>
cities first try november
</commit_message>
<xml_diff>
--- a/data/all_cards.xlsx
+++ b/data/all_cards.xlsx
@@ -495,9 +495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -680,7 +678,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -750,10 +748,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -890,10 +888,10 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -918,7 +916,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C30">
         <v>0</v>

</xml_diff>